<commit_message>
added two new columns in prompt
</commit_message>
<xml_diff>
--- a/src/dataset/gemini-zero-shot/Rahmatullah-Cr.MB.No.337-D-17.xlsx
+++ b/src/dataset/gemini-zero-shot/Rahmatullah-Cr.MB.No.337-D-17.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -427,6 +427,8 @@
     <col width="50" customWidth="1" min="1" max="1"/>
     <col width="50" customWidth="1" min="2" max="2"/>
     <col width="50" customWidth="1" min="3" max="3"/>
+    <col width="50" customWidth="1" min="4" max="4"/>
+    <col width="50" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -442,6 +444,16 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Prosecution Counsel Statement</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Defense Counsel Statement</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Judgment</t>
         </is>
       </c>
@@ -449,19 +461,13 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>** On 26.4.2017 at 1130 hours, complainant Salimullah Khan, SHO Police Station Gomal University, D.I.Khan, along with other police officials, conducted a search and strategic operation. While returning to the police station via Jhauk Ladho to Kat Shahani, Wilayat Khan DFC, Constable Javed Iqbal, Constable Mazhar and Constable Muhammad Ramzan were ahead on motorcycles, while the remaining police personnel followed in an official vehicle. Near the graveyard on the metaled road Kat Shahani, they encountered six unknown terrorists who opened indiscriminate fire, injuring Wilayat Khan DFC and Constable Javed Iqbal. The police returned fire in self-defense. The terrorists also threw hand grenades. Four terrorists fled, while two took refuge near a tube-well. Army personnel, QRF and CTD staff arrived, and the two terrorists blew themselves up. Recovered from the terrorists were two 9 MM pistols with magazines, live cartridges, and a live hand grenade. Three motorcycles parked at the spot were seized. FIR No.13 was registered under Sections 324/353/148/149 PPC read with Sections 3/4/5 of the Explosive Substances Act/ 7 of Anti-Terrorism Act, 1997 and 15 of Arms Act at Police Station C.T.D, D.I.Khan. The accused/petitioners, Rahmatullah and Rafiullah, were arrested in case FIR No.461 dated 22.10.2016 under Section 15 Arms Act of Police Station Gomal University, D.I-Khan and formally arrested in the instant case on the same day.</t>
-        </is>
-      </c>
-      <c r="B2" s="1" t="inlineStr">
-        <is>
-          <t>** *   **Allah Wasaya:** Gave a supplementary statement under Section 164 Cr.P.C on 21.6.2017, stating that Matiullah and Kashif Jamal alias Khalid (both killed in police encounter), Umer Farooq, and Rehmatullah were fast friends. He also stated there was a general rumor his son and other companions were involved in terrorist activities, and his son and relative Muhammad Javed had left the motorcycle on the spot.</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>** The court applied Section 497(2) Cr.P.C. The court allowed the criminal miscellaneous bail applications. The petitioners Rahmatullah and Rafiullah were directed to be released on bail subject to furnishing bail bonds of Rs. 5,00,000 each, with two sureties each of the like amount, to the satisfaction of the Illaqa/Duty Judicial Magistrate. **Findings of the court/Basis of decision:** The court found that sufficient incriminating material was lacking to connect the petitioners to the alleged offenses. The court noted the presumption of innocence and stated that the A.A.G. could not point to any incriminating material, except the statement of Allah Wasaya, which only indicated that the petitioners were friends with some of the terrorists and there was a rumor of their involvement. Mobile data did not disclose any contact between the petitioners and the terrorists at the time of the occurrence. The court held that the case fell within the ambit of further inquiry under Section 497(2) Cr.P.C. The court found that the prosecution version left much to be inquired into and it was not known how the alleged offense was abetted or facilitated by the petitioners. The court also analyzed Section 21-D(4) of the Anti-Terrorism Act 1997 and found no basis to apply it against the petitioners. The challan (report of the investigating officer) had not been submitted against the accused despite the case being registered on 26.4.2017.</t>
-        </is>
-      </c>
+          <t>** On 26.4.2017 at 1130 hours, police officials were returning to the police station after a search operation when they were attacked by six unknown terrorists near a graveyard. The terrorists opened fire and threw hand grenades, injuring two constables. The police returned fire. Four terrorists fled, while two remained and continued firing near a tube-well. Army personnel, QRF and CTD staff arrived, and the two remaining terrorists blew themselves up. Police recovered two 9mm pistols, live cartridges, and a hand grenade from the terrorists, and took possession of three motorcycles. FIR No.13 was registered under Sections 324/353/148/149 PPC, Sections 3/4/5 of the Explosive Substances Act, Section 7 of the Anti-Terrorism Act, 1997, and Section 15 of the Arms Act at Police Station C.T.D, D.I.Khan. Rahmatullah and Rafiullah were arrested in connection with the case while already in custody for another case (FIR No.461 dated 22.10.2016 under Section 15 Arms Act).</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr"/>
+      <c r="C2" s="1" t="inlineStr"/>
+      <c r="D2" s="1" t="inlineStr"/>
+      <c r="E2" s="1" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>